<commit_message>
adding laboratory data and fuzzy names for nmatch_dummy
</commit_message>
<xml_diff>
--- a/data/final/xlsx/moissala_laboratory_EN.xlsx
+++ b/data/final/xlsx/moissala_laboratory_EN.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E348"/>
+  <dimension ref="A1:E352"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -401,14 +401,11 @@
         </is>
       </c>
       <c r="C2" s="2">
-        <v>44789.73784676657</v>
-      </c>
-      <c r="D2">
-        <v>25.7</v>
+        <v>44788.73784676657</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -422,10 +419,10 @@
         </is>
       </c>
       <c r="C3" s="2">
-        <v>44822.03841206255</v>
+        <v>44823.03841206255</v>
       </c>
       <c r="D3">
-        <v>28.6</v>
+        <v>26.5</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -443,10 +440,10 @@
         </is>
       </c>
       <c r="C4" s="2">
-        <v>44834.69365665365</v>
+        <v>44833.69365665365</v>
       </c>
       <c r="D4">
-        <v>28</v>
+        <v>26.6</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -464,10 +461,10 @@
         </is>
       </c>
       <c r="C5" s="2">
-        <v>44839.67702252154</v>
+        <v>44838.67702252154</v>
       </c>
       <c r="D5">
-        <v>28.6</v>
+        <v>27</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -485,10 +482,10 @@
         </is>
       </c>
       <c r="C6" s="2">
-        <v>44831.99513009658</v>
+        <v>44830.99513009658</v>
       </c>
       <c r="D6">
-        <v>28.2</v>
+        <v>26.5</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -506,14 +503,11 @@
         </is>
       </c>
       <c r="C7" s="2">
-        <v>44842.76079000802</v>
-      </c>
-      <c r="D7">
-        <v>27.9</v>
+        <v>44843.76079000802</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -527,11 +521,14 @@
         </is>
       </c>
       <c r="C8" s="2">
-        <v>44857.15593130107</v>
+        <v>44854.15593130107</v>
+      </c>
+      <c r="D8">
+        <v>26.8</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -545,10 +542,10 @@
         </is>
       </c>
       <c r="C9" s="2">
-        <v>44852.3558266066</v>
+        <v>44851.3558266066</v>
       </c>
       <c r="D9">
-        <v>27.6</v>
+        <v>27.8</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -566,10 +563,10 @@
         </is>
       </c>
       <c r="C10" s="2">
-        <v>44862.30895245619</v>
+        <v>44861.30895245619</v>
       </c>
       <c r="D10">
-        <v>27.3</v>
+        <v>26.2</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -590,7 +587,7 @@
         <v>44877.97220562101</v>
       </c>
       <c r="D11">
-        <v>28.1</v>
+        <v>28</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -611,7 +608,7 @@
         <v>44874.94736973759</v>
       </c>
       <c r="D12">
-        <v>26.8</v>
+        <v>26.4</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -629,10 +626,10 @@
         </is>
       </c>
       <c r="C13" s="2">
-        <v>44879.87553108525</v>
+        <v>44878.87553108525</v>
       </c>
       <c r="D13">
-        <v>26.8</v>
+        <v>27.3</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -650,10 +647,10 @@
         </is>
       </c>
       <c r="C14" s="2">
-        <v>44904.66474369627</v>
+        <v>44906.66474369627</v>
       </c>
       <c r="D14">
-        <v>26.5</v>
+        <v>26.6</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -671,7 +668,7 @@
         </is>
       </c>
       <c r="C15" s="2">
-        <v>44903.73362138377</v>
+        <v>44901.73362138377</v>
       </c>
       <c r="D15">
         <v>27.9</v>
@@ -692,10 +689,10 @@
         </is>
       </c>
       <c r="C16" s="2">
-        <v>44882.67571101949</v>
+        <v>44881.67571101949</v>
       </c>
       <c r="D16">
-        <v>27.5</v>
+        <v>28.2</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -713,10 +710,10 @@
         </is>
       </c>
       <c r="C17" s="2">
-        <v>44897.54230103768</v>
+        <v>44898.54230103768</v>
       </c>
       <c r="D17">
-        <v>27.6</v>
+        <v>27.1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -734,10 +731,10 @@
         </is>
       </c>
       <c r="C18" s="2">
-        <v>44915.1849459402</v>
+        <v>44914.1849459402</v>
       </c>
       <c r="D18">
-        <v>27.6</v>
+        <v>26.9</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -755,14 +752,11 @@
         </is>
       </c>
       <c r="C19" s="2">
-        <v>44894.46156552874</v>
-      </c>
-      <c r="D19">
-        <v>29</v>
+        <v>44892.46156552874</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -776,10 +770,10 @@
         </is>
       </c>
       <c r="C20" s="2">
-        <v>44939.2116112354</v>
+        <v>44936.2116112354</v>
       </c>
       <c r="D20">
-        <v>26.2</v>
+        <v>27.6</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -797,14 +791,11 @@
         </is>
       </c>
       <c r="C21" s="2">
-        <v>44884.76500603766</v>
-      </c>
-      <c r="D21">
-        <v>28.2</v>
+        <v>44887.76500603766</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -818,7 +809,7 @@
         </is>
       </c>
       <c r="C22" s="2">
-        <v>44913.62103307399</v>
+        <v>44916.62103307399</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -836,10 +827,10 @@
         </is>
       </c>
       <c r="C23" s="2">
-        <v>44922.08509284106</v>
+        <v>44923.08509284106</v>
       </c>
       <c r="D23">
-        <v>29.4</v>
+        <v>26.6</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -857,10 +848,10 @@
         </is>
       </c>
       <c r="C24" s="2">
-        <v>44934.14061802191</v>
+        <v>44933.14061802191</v>
       </c>
       <c r="D24">
-        <v>27.6</v>
+        <v>28</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -878,10 +869,10 @@
         </is>
       </c>
       <c r="C25" s="2">
-        <v>44942.85287541537</v>
+        <v>44943.85287541537</v>
       </c>
       <c r="D25">
-        <v>27.1</v>
+        <v>27.7</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -899,10 +890,10 @@
         </is>
       </c>
       <c r="C26" s="2">
-        <v>44937.96017812754</v>
+        <v>44939.96017812754</v>
       </c>
       <c r="D26">
-        <v>26.6</v>
+        <v>27.2</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -920,10 +911,10 @@
         </is>
       </c>
       <c r="C27" s="2">
-        <v>44947.75033129116</v>
+        <v>44944.75033129116</v>
       </c>
       <c r="D27">
-        <v>27.3</v>
+        <v>26.5</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -941,10 +932,10 @@
         </is>
       </c>
       <c r="C28" s="2">
-        <v>44908.67587913231</v>
+        <v>44907.67587913231</v>
       </c>
       <c r="D28">
-        <v>26.4</v>
+        <v>26.6</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -965,7 +956,7 @@
         <v>44952.23151649674</v>
       </c>
       <c r="D29">
-        <v>27</v>
+        <v>27.4</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -983,10 +974,10 @@
         </is>
       </c>
       <c r="C30" s="2">
-        <v>44957.65639504021</v>
+        <v>44958.65639504021</v>
       </c>
       <c r="D30">
-        <v>27.8</v>
+        <v>25.6</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1004,10 +995,10 @@
         </is>
       </c>
       <c r="C31" s="2">
-        <v>44942.63929134344</v>
+        <v>44943.63929134344</v>
       </c>
       <c r="D31">
-        <v>26.4</v>
+        <v>26</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1025,11 +1016,14 @@
         </is>
       </c>
       <c r="C32" s="2">
-        <v>44949.21497790409</v>
+        <v>44947.21497790409</v>
+      </c>
+      <c r="D32">
+        <v>28.1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1043,10 +1037,10 @@
         </is>
       </c>
       <c r="C33" s="2">
-        <v>44957.33290892333</v>
+        <v>44955.33290892333</v>
       </c>
       <c r="D33">
-        <v>26.7</v>
+        <v>27.7</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1064,10 +1058,10 @@
         </is>
       </c>
       <c r="C34" s="2">
-        <v>44952.84720995915</v>
+        <v>44950.84720995915</v>
       </c>
       <c r="D34">
-        <v>27</v>
+        <v>25.9</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1085,14 +1079,11 @@
         </is>
       </c>
       <c r="C35" s="2">
-        <v>44969.19165913553</v>
-      </c>
-      <c r="D35">
-        <v>26.3</v>
+        <v>44970.19165913553</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -1106,10 +1097,10 @@
         </is>
       </c>
       <c r="C36" s="2">
-        <v>44958.86994735798</v>
+        <v>44959.86994735798</v>
       </c>
       <c r="D36">
-        <v>29.1</v>
+        <v>28</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1127,14 +1118,11 @@
         </is>
       </c>
       <c r="C37" s="2">
-        <v>44963.45561075702</v>
-      </c>
-      <c r="D37">
-        <v>26.1</v>
+        <v>44966.45561075702</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -1148,10 +1136,10 @@
         </is>
       </c>
       <c r="C38" s="2">
-        <v>44966.36158320674</v>
+        <v>44968.36158320674</v>
       </c>
       <c r="D38">
-        <v>27.1</v>
+        <v>28.5</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1172,7 +1160,7 @@
         <v>44970.08325492992</v>
       </c>
       <c r="D39">
-        <v>26.6</v>
+        <v>27.4</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1190,10 +1178,10 @@
         </is>
       </c>
       <c r="C40" s="2">
-        <v>44962.4243041155</v>
+        <v>44959.4243041155</v>
       </c>
       <c r="D40">
-        <v>27.7</v>
+        <v>27.1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1214,7 +1202,7 @@
         <v>44975.8973325459</v>
       </c>
       <c r="D41">
-        <v>27.6</v>
+        <v>27.4</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1232,10 +1220,10 @@
         </is>
       </c>
       <c r="C42" s="2">
-        <v>44984.8177446101</v>
+        <v>44983.8177446101</v>
       </c>
       <c r="D42">
-        <v>26.5</v>
+        <v>26.1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1256,7 +1244,7 @@
         <v>44972.4262226739</v>
       </c>
       <c r="D43">
-        <v>27.8</v>
+        <v>27.6</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1274,10 +1262,10 @@
         </is>
       </c>
       <c r="C44" s="2">
-        <v>44969.4244591125</v>
+        <v>44968.4244591125</v>
       </c>
       <c r="D44">
-        <v>27.5</v>
+        <v>26.8</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1295,14 +1283,11 @@
         </is>
       </c>
       <c r="C45" s="2">
-        <v>44974.559348137</v>
-      </c>
-      <c r="D45">
-        <v>28.5</v>
+        <v>44975.559348137</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -1316,11 +1301,14 @@
         </is>
       </c>
       <c r="C46" s="2">
-        <v>44991.74936818991</v>
+        <v>44992.74936818991</v>
+      </c>
+      <c r="D46">
+        <v>27.5</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1334,11 +1322,14 @@
         </is>
       </c>
       <c r="C47" s="2">
-        <v>44985.22862544721</v>
+        <v>44988.22862544721</v>
+      </c>
+      <c r="D47">
+        <v>27.1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1352,10 +1343,10 @@
         </is>
       </c>
       <c r="C48" s="2">
-        <v>44994.28225565708</v>
+        <v>44997.28225565708</v>
       </c>
       <c r="D48">
-        <v>27.9</v>
+        <v>27</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1373,10 +1364,10 @@
         </is>
       </c>
       <c r="C49" s="2">
-        <v>44993.22218131204</v>
+        <v>44992.22218131204</v>
       </c>
       <c r="D49">
-        <v>27.5</v>
+        <v>27.8</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1394,10 +1385,10 @@
         </is>
       </c>
       <c r="C50" s="2">
-        <v>44993.06691476925</v>
+        <v>44995.06691476925</v>
       </c>
       <c r="D50">
-        <v>26.9</v>
+        <v>26.7</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1417,9 +1408,12 @@
       <c r="C51" s="2">
         <v>44975.5566737184</v>
       </c>
+      <c r="D51">
+        <v>26</v>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1433,10 +1427,10 @@
         </is>
       </c>
       <c r="C52" s="2">
-        <v>44992.2995246853</v>
+        <v>44990.2995246853</v>
       </c>
       <c r="D52">
-        <v>27.3</v>
+        <v>28.1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1454,7 +1448,7 @@
         </is>
       </c>
       <c r="C53" s="2">
-        <v>45015.82999534273</v>
+        <v>45014.82999534273</v>
       </c>
       <c r="D53">
         <v>26.9</v>
@@ -1475,10 +1469,10 @@
         </is>
       </c>
       <c r="C54" s="2">
-        <v>44987.29123377963</v>
+        <v>44988.29123377963</v>
       </c>
       <c r="D54">
-        <v>27.8</v>
+        <v>28.5</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1496,10 +1490,10 @@
         </is>
       </c>
       <c r="C55" s="2">
-        <v>44996.21024860656</v>
+        <v>44997.21024860656</v>
       </c>
       <c r="D55">
-        <v>25.5</v>
+        <v>24.2</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1517,10 +1511,10 @@
         </is>
       </c>
       <c r="C56" s="2">
-        <v>45001.43131408491</v>
+        <v>44999.43131408491</v>
       </c>
       <c r="D56">
-        <v>27.7</v>
+        <v>27</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1538,10 +1532,10 @@
         </is>
       </c>
       <c r="C57" s="2">
-        <v>45011.27813154997</v>
+        <v>45010.27813154997</v>
       </c>
       <c r="D57">
-        <v>28.1</v>
+        <v>27.8</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1559,10 +1553,10 @@
         </is>
       </c>
       <c r="C58" s="2">
-        <v>44987.54287277162</v>
+        <v>44989.54287277162</v>
       </c>
       <c r="D58">
-        <v>27.8</v>
+        <v>27.3</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1583,7 +1577,7 @@
         <v>45016.74035197373</v>
       </c>
       <c r="D59">
-        <v>24.9</v>
+        <v>28.9</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1604,7 +1598,7 @@
         <v>45001.7263564133</v>
       </c>
       <c r="D60">
-        <v>28.8</v>
+        <v>27.8</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1622,10 +1616,10 @@
         </is>
       </c>
       <c r="C61" s="2">
-        <v>45010.13201330748</v>
+        <v>45008.13201330748</v>
       </c>
       <c r="D61">
-        <v>27.5</v>
+        <v>27</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1645,9 +1639,12 @@
       <c r="C62" s="2">
         <v>45013.14444656829</v>
       </c>
+      <c r="D62">
+        <v>26.1</v>
+      </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1664,7 +1661,7 @@
         <v>45003.25170763618</v>
       </c>
       <c r="D63">
-        <v>24.9</v>
+        <v>26.1</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1682,14 +1679,11 @@
         </is>
       </c>
       <c r="C64" s="2">
-        <v>45022.60309603589</v>
-      </c>
-      <c r="D64">
-        <v>24.2</v>
+        <v>45019.60309603589</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -1703,10 +1697,10 @@
         </is>
       </c>
       <c r="C65" s="2">
-        <v>45020.23782132017</v>
+        <v>45019.23782132017</v>
       </c>
       <c r="D65">
-        <v>26.7</v>
+        <v>27.5</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1726,12 +1720,9 @@
       <c r="C66" s="2">
         <v>45008.18506884721</v>
       </c>
-      <c r="D66">
-        <v>27.4</v>
-      </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -1745,11 +1736,14 @@
         </is>
       </c>
       <c r="C67" s="2">
-        <v>45014.51728321377</v>
+        <v>45016.51728321377</v>
+      </c>
+      <c r="D67">
+        <v>26.6</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1766,7 +1760,7 @@
         <v>45012.90726379526</v>
       </c>
       <c r="D68">
-        <v>25.5</v>
+        <v>26.5</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -1784,11 +1778,14 @@
         </is>
       </c>
       <c r="C69" s="2">
-        <v>44981.86667364836</v>
+        <v>44982.86667364836</v>
+      </c>
+      <c r="D69">
+        <v>26.5</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1802,10 +1799,10 @@
         </is>
       </c>
       <c r="C70" s="2">
-        <v>45016.48488610215</v>
+        <v>45019.48488610215</v>
       </c>
       <c r="D70">
-        <v>27.5</v>
+        <v>27.3</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -1825,9 +1822,12 @@
       <c r="C71" s="2">
         <v>45021.68565493632</v>
       </c>
+      <c r="D71">
+        <v>28.4</v>
+      </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1843,12 +1843,9 @@
       <c r="C72" s="2">
         <v>45028.75037402037</v>
       </c>
-      <c r="D72">
-        <v>27.9</v>
-      </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -1862,10 +1859,10 @@
         </is>
       </c>
       <c r="C73" s="2">
-        <v>45026.76628873566</v>
+        <v>45029.76628873566</v>
       </c>
       <c r="D73">
-        <v>27.9</v>
+        <v>27.8</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -1883,10 +1880,10 @@
         </is>
       </c>
       <c r="C74" s="2">
-        <v>45012.08445902637</v>
+        <v>45010.08445902637</v>
       </c>
       <c r="D74">
-        <v>27</v>
+        <v>28.5</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -1904,11 +1901,14 @@
         </is>
       </c>
       <c r="C75" s="2">
-        <v>45017.6025040252</v>
+        <v>45016.6025040252</v>
+      </c>
+      <c r="D75">
+        <v>28.4</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
         <v>45033.19920331283</v>
       </c>
       <c r="D76">
-        <v>27</v>
+        <v>26.6</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -1943,10 +1943,10 @@
         </is>
       </c>
       <c r="C77" s="2">
-        <v>45026.77221659505</v>
+        <v>45028.77221659505</v>
       </c>
       <c r="D77">
-        <v>27.5</v>
+        <v>27</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -1964,11 +1964,14 @@
         </is>
       </c>
       <c r="C78" s="2">
-        <v>45005.60016729333</v>
+        <v>45007.60016729333</v>
+      </c>
+      <c r="D78">
+        <v>27</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1988,7 @@
         <v>45001.81880240295</v>
       </c>
       <c r="D79">
-        <v>27.1</v>
+        <v>27.4</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2003,10 +2006,10 @@
         </is>
       </c>
       <c r="C80" s="2">
-        <v>45018.78346967344</v>
+        <v>45015.78346967344</v>
       </c>
       <c r="D80">
-        <v>26.2</v>
+        <v>28.2</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2024,14 +2027,11 @@
         </is>
       </c>
       <c r="C81" s="2">
-        <v>45041.00957551961</v>
-      </c>
-      <c r="D81">
-        <v>27.2</v>
+        <v>45044.00957551961</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -2045,11 +2045,14 @@
         </is>
       </c>
       <c r="C82" s="2">
-        <v>45005.15511983701</v>
+        <v>45003.15511983701</v>
+      </c>
+      <c r="D82">
+        <v>24.9</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2063,10 +2066,10 @@
         </is>
       </c>
       <c r="C83" s="2">
-        <v>45021.58446043505</v>
+        <v>45020.58446043505</v>
       </c>
       <c r="D83">
-        <v>27.8</v>
+        <v>27.3</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2084,10 +2087,10 @@
         </is>
       </c>
       <c r="C84" s="2">
-        <v>45055.42828921101</v>
+        <v>45056.42828921101</v>
       </c>
       <c r="D84">
-        <v>27.7</v>
+        <v>28.3</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2108,7 +2111,7 @@
         <v>45046.32751682845</v>
       </c>
       <c r="D85">
-        <v>27.8</v>
+        <v>26.8</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2126,10 +2129,10 @@
         </is>
       </c>
       <c r="C86" s="2">
-        <v>45039.17498208776</v>
+        <v>45040.17498208776</v>
       </c>
       <c r="D86">
-        <v>27.5</v>
+        <v>27.4</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2147,10 +2150,10 @@
         </is>
       </c>
       <c r="C87" s="2">
-        <v>45022.79310166626</v>
+        <v>45024.79310166626</v>
       </c>
       <c r="D87">
-        <v>28.1</v>
+        <v>25.6</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2168,10 +2171,10 @@
         </is>
       </c>
       <c r="C88" s="2">
-        <v>45020.35716133921</v>
+        <v>45017.35716133921</v>
       </c>
       <c r="D88">
-        <v>28.8</v>
+        <v>26.5</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2189,7 +2192,7 @@
         </is>
       </c>
       <c r="C89" s="2">
-        <v>45018.7135926999</v>
+        <v>45016.7135926999</v>
       </c>
       <c r="D89">
         <v>27.7</v>
@@ -2210,10 +2213,10 @@
         </is>
       </c>
       <c r="C90" s="2">
-        <v>45030.63805744599</v>
+        <v>45033.63805744599</v>
       </c>
       <c r="D90">
-        <v>29.2</v>
+        <v>26.9</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2231,11 +2234,14 @@
         </is>
       </c>
       <c r="C91" s="2">
-        <v>45041.52050106211</v>
+        <v>45039.52050106211</v>
+      </c>
+      <c r="D91">
+        <v>25.1</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2249,7 +2255,7 @@
         </is>
       </c>
       <c r="C92" s="2">
-        <v>45005.23590839887</v>
+        <v>45006.23590839887</v>
       </c>
       <c r="D92">
         <v>26.7</v>
@@ -2270,10 +2276,10 @@
         </is>
       </c>
       <c r="C93" s="2">
-        <v>45052.67994101599</v>
+        <v>45054.67994101599</v>
       </c>
       <c r="D93">
-        <v>27.9</v>
+        <v>28.4</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2294,7 +2300,7 @@
         <v>45002.31012779978</v>
       </c>
       <c r="D94">
-        <v>24.8</v>
+        <v>27.8</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2314,12 +2320,9 @@
       <c r="C95" s="2">
         <v>45017.90476873251</v>
       </c>
-      <c r="D95">
-        <v>26.5</v>
-      </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -2333,10 +2336,10 @@
         </is>
       </c>
       <c r="C96" s="2">
-        <v>45009.36978730019</v>
+        <v>45008.36978730019</v>
       </c>
       <c r="D96">
-        <v>26.9</v>
+        <v>27.4</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2354,11 +2357,14 @@
         </is>
       </c>
       <c r="C97" s="2">
-        <v>45042.44525145847</v>
+        <v>45041.44525145847</v>
+      </c>
+      <c r="D97">
+        <v>29.4</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2372,10 +2378,10 @@
         </is>
       </c>
       <c r="C98" s="2">
-        <v>45063.43920018859</v>
+        <v>45065.43920018859</v>
       </c>
       <c r="D98">
-        <v>27.8</v>
+        <v>27.7</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2393,10 +2399,10 @@
         </is>
       </c>
       <c r="C99" s="2">
-        <v>45055.88395037441</v>
+        <v>45054.88395037441</v>
       </c>
       <c r="D99">
-        <v>27.3</v>
+        <v>25.4</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2417,7 +2423,7 @@
         <v>45067.92707325395</v>
       </c>
       <c r="D100">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2438,7 +2444,7 @@
         <v>45018.66953112079</v>
       </c>
       <c r="D101">
-        <v>28.1</v>
+        <v>25.1</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2456,10 +2462,10 @@
         </is>
       </c>
       <c r="C102" s="2">
-        <v>45016.23790423319</v>
+        <v>45017.23790423319</v>
       </c>
       <c r="D102">
-        <v>30.8</v>
+        <v>27.2</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2477,10 +2483,10 @@
         </is>
       </c>
       <c r="C103" s="2">
-        <v>45015.52530873661</v>
+        <v>45014.52530873661</v>
       </c>
       <c r="D103">
-        <v>26.5</v>
+        <v>25.1</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2501,7 +2507,7 @@
         <v>45042.83996908816</v>
       </c>
       <c r="D104">
-        <v>25.3</v>
+        <v>28.9</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2522,7 +2528,7 @@
         <v>45071.01530373779</v>
       </c>
       <c r="D105">
-        <v>26.6</v>
+        <v>29.1</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2540,10 +2546,10 @@
         </is>
       </c>
       <c r="C106" s="2">
-        <v>45028.26664946554</v>
+        <v>45029.26664946554</v>
       </c>
       <c r="D106">
-        <v>27.8</v>
+        <v>30</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -2561,7 +2567,7 @@
         </is>
       </c>
       <c r="C107" s="2">
-        <v>45047.96031026218</v>
+        <v>45049.96031026218</v>
       </c>
       <c r="D107">
         <v>27.2</v>
@@ -2582,14 +2588,11 @@
         </is>
       </c>
       <c r="C108" s="2">
-        <v>45064.34530363378</v>
-      </c>
-      <c r="D108">
-        <v>28.3</v>
+        <v>45065.34530363378</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -2603,10 +2606,10 @@
         </is>
       </c>
       <c r="C109" s="2">
-        <v>45057.24492114753</v>
+        <v>45059.24492114753</v>
       </c>
       <c r="D109">
-        <v>26.8</v>
+        <v>28.1</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -2624,10 +2627,10 @@
         </is>
       </c>
       <c r="C110" s="2">
-        <v>45075.13800457637</v>
+        <v>45076.13800457637</v>
       </c>
       <c r="D110">
-        <v>26.6</v>
+        <v>27.9</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -2645,10 +2648,10 @@
         </is>
       </c>
       <c r="C111" s="2">
-        <v>45019.51805158485</v>
+        <v>45020.51805158485</v>
       </c>
       <c r="D111">
-        <v>25.6</v>
+        <v>26.4</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -2666,14 +2669,11 @@
         </is>
       </c>
       <c r="C112" s="2">
-        <v>45038.32752088627</v>
-      </c>
-      <c r="D112">
-        <v>24.6</v>
+        <v>45039.32752088627</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -2687,10 +2687,10 @@
         </is>
       </c>
       <c r="C113" s="2">
-        <v>45038.95270198777</v>
+        <v>45036.95270198777</v>
       </c>
       <c r="D113">
-        <v>24.4</v>
+        <v>26.9</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -2708,10 +2708,10 @@
         </is>
       </c>
       <c r="C114" s="2">
-        <v>45032.88074707224</v>
+        <v>45031.88074707224</v>
       </c>
       <c r="D114">
-        <v>26.9</v>
+        <v>27.9</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -2729,10 +2729,10 @@
         </is>
       </c>
       <c r="C115" s="2">
-        <v>45032.99808206191</v>
+        <v>45030.99808206191</v>
       </c>
       <c r="D115">
-        <v>28.3</v>
+        <v>27.6</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -2752,9 +2752,12 @@
       <c r="C116" s="2">
         <v>45065.67696978927</v>
       </c>
+      <c r="D116">
+        <v>28</v>
+      </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2768,10 +2771,10 @@
         </is>
       </c>
       <c r="C117" s="2">
-        <v>45051.529365629</v>
+        <v>45049.529365629</v>
       </c>
       <c r="D117">
-        <v>25.6</v>
+        <v>27.6</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -2789,11 +2792,14 @@
         </is>
       </c>
       <c r="C118" s="2">
-        <v>45053.97612192866</v>
+        <v>45054.97612192866</v>
+      </c>
+      <c r="D118">
+        <v>26</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2810,7 +2816,7 @@
         <v>45067.67823733149</v>
       </c>
       <c r="D119">
-        <v>27.8</v>
+        <v>26.9</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -2828,10 +2834,10 @@
         </is>
       </c>
       <c r="C120" s="2">
-        <v>45049.49110184248</v>
+        <v>45051.49110184248</v>
       </c>
       <c r="D120">
-        <v>26</v>
+        <v>27.5</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -2849,10 +2855,10 @@
         </is>
       </c>
       <c r="C121" s="2">
-        <v>45058.08072278915</v>
+        <v>45061.08072278915</v>
       </c>
       <c r="D121">
-        <v>25.5</v>
+        <v>27.2</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -2872,9 +2878,12 @@
       <c r="C122" s="2">
         <v>45064.57257599347</v>
       </c>
+      <c r="D122">
+        <v>25.4</v>
+      </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2888,14 +2897,11 @@
         </is>
       </c>
       <c r="C123" s="2">
-        <v>45078.29387128746</v>
-      </c>
-      <c r="D123">
-        <v>27.2</v>
+        <v>45081.29387128746</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -2909,7 +2915,7 @@
         </is>
       </c>
       <c r="C124" s="2">
-        <v>45070.25890073265</v>
+        <v>45072.25890073265</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -2929,12 +2935,9 @@
       <c r="C125" s="2">
         <v>45063.23959472299</v>
       </c>
-      <c r="D125">
-        <v>26.7</v>
-      </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -2948,14 +2951,11 @@
         </is>
       </c>
       <c r="C126" s="2">
-        <v>45038.65592720595</v>
-      </c>
-      <c r="D126">
-        <v>27</v>
+        <v>45037.65592720595</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -2969,10 +2969,10 @@
         </is>
       </c>
       <c r="C127" s="2">
-        <v>45050.10467578134</v>
+        <v>45052.10467578134</v>
       </c>
       <c r="D127">
-        <v>25.8</v>
+        <v>27.4</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -2990,10 +2990,10 @@
         </is>
       </c>
       <c r="C128" s="2">
-        <v>45057.30476006951</v>
+        <v>45058.30476006951</v>
       </c>
       <c r="D128">
-        <v>28.2</v>
+        <v>28.5</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3011,7 +3011,7 @@
         </is>
       </c>
       <c r="C129" s="2">
-        <v>45091.08761669937</v>
+        <v>45092.08761669937</v>
       </c>
       <c r="D129">
         <v>26.8</v>
@@ -3032,10 +3032,10 @@
         </is>
       </c>
       <c r="C130" s="2">
-        <v>45054.57918735305</v>
+        <v>45055.57918735305</v>
       </c>
       <c r="D130">
-        <v>26.8</v>
+        <v>27.8</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3053,10 +3053,10 @@
         </is>
       </c>
       <c r="C131" s="2">
-        <v>45082.51780517718</v>
+        <v>45084.51780517718</v>
       </c>
       <c r="D131">
-        <v>27.2</v>
+        <v>26.3</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3074,14 +3074,11 @@
         </is>
       </c>
       <c r="C132" s="2">
-        <v>45070.70593476942</v>
-      </c>
-      <c r="D132">
-        <v>27.1</v>
+        <v>45072.70593476942</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -3095,11 +3092,14 @@
         </is>
       </c>
       <c r="C133" s="2">
-        <v>45056.9382756232</v>
+        <v>45054.9382756232</v>
+      </c>
+      <c r="D133">
+        <v>26.9</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3113,10 +3113,10 @@
         </is>
       </c>
       <c r="C134" s="2">
-        <v>45059.71488302403</v>
+        <v>45057.71488302403</v>
       </c>
       <c r="D134">
-        <v>28</v>
+        <v>29.2</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3134,10 +3134,10 @@
         </is>
       </c>
       <c r="C135" s="2">
-        <v>45076.06268669991</v>
+        <v>45074.06268669991</v>
       </c>
       <c r="D135">
-        <v>27.2</v>
+        <v>27.4</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3155,10 +3155,10 @@
         </is>
       </c>
       <c r="C136" s="2">
-        <v>45076.66785892371</v>
+        <v>45078.66785892371</v>
       </c>
       <c r="D136">
-        <v>26.2</v>
+        <v>28.1</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3176,10 +3176,10 @@
         </is>
       </c>
       <c r="C137" s="2">
-        <v>45117.02984727934</v>
+        <v>45115.02984727934</v>
       </c>
       <c r="D137">
-        <v>26.9</v>
+        <v>28.1</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3197,10 +3197,10 @@
         </is>
       </c>
       <c r="C138" s="2">
-        <v>45113.58818697675</v>
+        <v>45112.58818697675</v>
       </c>
       <c r="D138">
-        <v>26.6</v>
+        <v>27.8</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3221,7 +3221,7 @@
         <v>45106.63150799398</v>
       </c>
       <c r="D139">
-        <v>26.8</v>
+        <v>27.8</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3239,10 +3239,10 @@
         </is>
       </c>
       <c r="C140" s="2">
-        <v>45080.62354923787</v>
+        <v>45079.62354923787</v>
       </c>
       <c r="D140">
-        <v>27.9</v>
+        <v>26.6</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3260,10 +3260,10 @@
         </is>
       </c>
       <c r="C141" s="2">
-        <v>45106.24501113055</v>
+        <v>45105.24501113055</v>
       </c>
       <c r="D141">
-        <v>26.3</v>
+        <v>27.3</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3281,11 +3281,14 @@
         </is>
       </c>
       <c r="C142" s="2">
-        <v>45110.33771034843</v>
+        <v>45109.33771034843</v>
+      </c>
+      <c r="D142">
+        <v>27.7</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3299,10 +3302,10 @@
         </is>
       </c>
       <c r="C143" s="2">
-        <v>45085.84102773334</v>
+        <v>45086.84102773334</v>
       </c>
       <c r="D143">
-        <v>25</v>
+        <v>27.5</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3320,14 +3323,11 @@
         </is>
       </c>
       <c r="C144" s="2">
-        <v>45079.58228165382</v>
-      </c>
-      <c r="D144">
-        <v>29.2</v>
+        <v>45078.58228165382</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -3341,10 +3341,10 @@
         </is>
       </c>
       <c r="C145" s="2">
-        <v>45084.74524194817</v>
+        <v>45081.74524194817</v>
       </c>
       <c r="D145">
-        <v>28.1</v>
+        <v>26.2</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3362,10 +3362,10 @@
         </is>
       </c>
       <c r="C146" s="2">
-        <v>45115.34001555393</v>
+        <v>45114.34001555393</v>
       </c>
       <c r="D146">
-        <v>28.1</v>
+        <v>27.5</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -3383,14 +3383,11 @@
         </is>
       </c>
       <c r="C147" s="2">
-        <v>45117.9699830747</v>
-      </c>
-      <c r="D147">
-        <v>27.4</v>
+        <v>45114.9699830747</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -3404,10 +3401,10 @@
         </is>
       </c>
       <c r="C148" s="2">
-        <v>45109.80560884319</v>
+        <v>45110.80560884319</v>
       </c>
       <c r="D148">
-        <v>27.5</v>
+        <v>27.8</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -3425,11 +3422,14 @@
         </is>
       </c>
       <c r="C149" s="2">
-        <v>45129.40256878556</v>
+        <v>45127.40256878556</v>
+      </c>
+      <c r="D149">
+        <v>27.4</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3443,10 +3443,10 @@
         </is>
       </c>
       <c r="C150" s="2">
-        <v>45077.67596857343</v>
+        <v>45079.67596857343</v>
       </c>
       <c r="D150">
-        <v>27.8</v>
+        <v>26.6</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -3464,14 +3464,11 @@
         </is>
       </c>
       <c r="C151" s="2">
-        <v>45117.29358809628</v>
-      </c>
-      <c r="D151">
-        <v>28.8</v>
+        <v>45118.29358809628</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -3485,10 +3482,10 @@
         </is>
       </c>
       <c r="C152" s="2">
-        <v>45108.96812768656</v>
+        <v>45109.96812768656</v>
       </c>
       <c r="D152">
-        <v>26.9</v>
+        <v>26.3</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -3508,12 +3505,9 @@
       <c r="C153" s="2">
         <v>45111.96701374761</v>
       </c>
-      <c r="D153">
-        <v>29</v>
-      </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -3527,14 +3521,11 @@
         </is>
       </c>
       <c r="C154" s="2">
-        <v>45122.17916409774</v>
-      </c>
-      <c r="D154">
-        <v>26.6</v>
+        <v>45124.17916409774</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -3548,10 +3539,10 @@
         </is>
       </c>
       <c r="C155" s="2">
-        <v>45119.90000550284</v>
+        <v>45121.90000550284</v>
       </c>
       <c r="D155">
-        <v>27.5</v>
+        <v>28</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -3569,10 +3560,10 @@
         </is>
       </c>
       <c r="C156" s="2">
-        <v>45125.57061823789</v>
+        <v>45126.57061823789</v>
       </c>
       <c r="D156">
-        <v>27.3</v>
+        <v>28.1</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -3590,10 +3581,10 @@
         </is>
       </c>
       <c r="C157" s="2">
-        <v>45122.90989141607</v>
+        <v>45121.90989141607</v>
       </c>
       <c r="D157">
-        <v>26.7</v>
+        <v>24.5</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -3611,10 +3602,10 @@
         </is>
       </c>
       <c r="C158" s="2">
-        <v>45127.41877833285</v>
+        <v>45125.41877833285</v>
       </c>
       <c r="D158">
-        <v>27.9</v>
+        <v>28.5</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -3632,10 +3623,10 @@
         </is>
       </c>
       <c r="C159" s="2">
-        <v>45119.9549940805</v>
+        <v>45118.9549940805</v>
       </c>
       <c r="D159">
-        <v>27.5</v>
+        <v>27.6</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -3656,7 +3647,7 @@
         <v>45121.83389702425</v>
       </c>
       <c r="D160">
-        <v>28.6</v>
+        <v>26.6</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -3674,14 +3665,11 @@
         </is>
       </c>
       <c r="C161" s="2">
-        <v>45070.38049159301</v>
-      </c>
-      <c r="D161">
-        <v>28.1</v>
+        <v>45069.38049159301</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -3695,10 +3683,10 @@
         </is>
       </c>
       <c r="C162" s="2">
-        <v>45127.85216800496</v>
+        <v>45126.85216800496</v>
       </c>
       <c r="D162">
-        <v>27.4</v>
+        <v>26.5</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -3719,7 +3707,7 @@
         <v>45133.45944308456</v>
       </c>
       <c r="D163">
-        <v>29.8</v>
+        <v>27</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -3737,10 +3725,10 @@
         </is>
       </c>
       <c r="C164" s="2">
-        <v>45131.43867306403</v>
+        <v>45132.43867306403</v>
       </c>
       <c r="D164">
-        <v>28.8</v>
+        <v>27</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -3758,10 +3746,10 @@
         </is>
       </c>
       <c r="C165" s="2">
-        <v>45102.36469465021</v>
+        <v>45101.36469465021</v>
       </c>
       <c r="D165">
-        <v>27.2</v>
+        <v>26.7</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -3779,10 +3767,10 @@
         </is>
       </c>
       <c r="C166" s="2">
-        <v>45143.69847920792</v>
+        <v>45145.69847920792</v>
       </c>
       <c r="D166">
-        <v>25.6</v>
+        <v>28</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -3800,10 +3788,10 @@
         </is>
       </c>
       <c r="C167" s="2">
-        <v>45143.25056248654</v>
+        <v>45141.25056248654</v>
       </c>
       <c r="D167">
-        <v>26.2</v>
+        <v>27.6</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -3821,10 +3809,10 @@
         </is>
       </c>
       <c r="C168" s="2">
-        <v>45155.66460960531</v>
+        <v>45156.66460960531</v>
       </c>
       <c r="D168">
-        <v>26.5</v>
+        <v>27.1</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -3842,14 +3830,11 @@
         </is>
       </c>
       <c r="C169" s="2">
-        <v>45101.75201548438</v>
-      </c>
-      <c r="D169">
-        <v>27</v>
+        <v>45100.75201548438</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -3863,10 +3848,10 @@
         </is>
       </c>
       <c r="C170" s="2">
-        <v>45139.77859537682</v>
+        <v>45140.77859537682</v>
       </c>
       <c r="D170">
-        <v>26.8</v>
+        <v>26.9</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -3884,10 +3869,10 @@
         </is>
       </c>
       <c r="C171" s="2">
-        <v>45093.72357663578</v>
+        <v>45094.72357663578</v>
       </c>
       <c r="D171">
-        <v>28.1</v>
+        <v>27.4</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -3905,10 +3890,10 @@
         </is>
       </c>
       <c r="C172" s="2">
-        <v>45101.98420643713</v>
+        <v>45102.98420643713</v>
       </c>
       <c r="D172">
-        <v>27.3</v>
+        <v>28.1</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -3926,10 +3911,10 @@
         </is>
       </c>
       <c r="C173" s="2">
-        <v>45108.9089936063</v>
+        <v>45107.9089936063</v>
       </c>
       <c r="D173">
-        <v>26.6</v>
+        <v>27.7</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -3947,10 +3932,10 @@
         </is>
       </c>
       <c r="C174" s="2">
-        <v>45109.44397149853</v>
+        <v>45110.44397149853</v>
       </c>
       <c r="D174">
-        <v>28.6</v>
+        <v>26.8</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -3968,10 +3953,10 @@
         </is>
       </c>
       <c r="C175" s="2">
-        <v>45105.35575637274</v>
+        <v>45106.35575637274</v>
       </c>
       <c r="D175">
-        <v>26.8</v>
+        <v>27.3</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -3989,10 +3974,10 @@
         </is>
       </c>
       <c r="C176" s="2">
-        <v>45161.31698659748</v>
+        <v>45162.31698659748</v>
       </c>
       <c r="D176">
-        <v>27.1</v>
+        <v>29</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4010,11 +3995,11 @@
         </is>
       </c>
       <c r="C177" s="2">
-        <v>45108.57957767218</v>
+        <v>45107.57957767218</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -4028,10 +4013,10 @@
         </is>
       </c>
       <c r="C178" s="2">
-        <v>45149.71824337228</v>
+        <v>45148.71824337228</v>
       </c>
       <c r="D178">
-        <v>27</v>
+        <v>26.9</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4052,7 +4037,7 @@
         <v>45151.97847126181</v>
       </c>
       <c r="D179">
-        <v>27.5</v>
+        <v>28.2</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4072,12 +4057,9 @@
       <c r="C180" s="2">
         <v>45148.91435035678</v>
       </c>
-      <c r="D180">
-        <v>25.8</v>
-      </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -4091,14 +4073,11 @@
         </is>
       </c>
       <c r="C181" s="2">
-        <v>45152.35639856065</v>
-      </c>
-      <c r="D181">
-        <v>26.4</v>
+        <v>45151.35639856065</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -4112,14 +4091,11 @@
         </is>
       </c>
       <c r="C182" s="2">
-        <v>45156.48530424261</v>
-      </c>
-      <c r="D182">
-        <v>27.1</v>
+        <v>45157.48530424261</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -4136,7 +4112,7 @@
         <v>45152.78717173701</v>
       </c>
       <c r="D183">
-        <v>27.1</v>
+        <v>28.1</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4154,10 +4130,10 @@
         </is>
       </c>
       <c r="C184" s="2">
-        <v>45153.11788901115</v>
+        <v>45151.11788901115</v>
       </c>
       <c r="D184">
-        <v>27.5</v>
+        <v>27.7</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4175,10 +4151,10 @@
         </is>
       </c>
       <c r="C185" s="2">
-        <v>45153.42694305828</v>
+        <v>45151.42694305828</v>
       </c>
       <c r="D185">
-        <v>27.2</v>
+        <v>28</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4196,10 +4172,10 @@
         </is>
       </c>
       <c r="C186" s="2">
-        <v>45098.53527948123</v>
+        <v>45100.53527948123</v>
       </c>
       <c r="D186">
-        <v>27.1</v>
+        <v>27</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -4217,10 +4193,10 @@
         </is>
       </c>
       <c r="C187" s="2">
-        <v>45161.29320304199</v>
+        <v>45163.29320304199</v>
       </c>
       <c r="D187">
-        <v>26.3</v>
+        <v>27.9</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -4238,10 +4214,10 @@
         </is>
       </c>
       <c r="C188" s="2">
-        <v>45149.28038766477</v>
+        <v>45150.28038766477</v>
       </c>
       <c r="D188">
-        <v>27</v>
+        <v>27.6</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -4259,10 +4235,10 @@
         </is>
       </c>
       <c r="C189" s="2">
-        <v>45157.34789422687</v>
+        <v>45159.34789422687</v>
       </c>
       <c r="D189">
-        <v>26.3</v>
+        <v>26.9</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -4280,14 +4256,11 @@
         </is>
       </c>
       <c r="C190" s="2">
-        <v>45146.96254063725</v>
-      </c>
-      <c r="D190">
-        <v>28.2</v>
+        <v>45147.96254063725</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -4301,10 +4274,10 @@
         </is>
       </c>
       <c r="C191" s="2">
-        <v>45163.90853975922</v>
+        <v>45162.90853975922</v>
       </c>
       <c r="D191">
-        <v>27.4</v>
+        <v>28.7</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -4322,10 +4295,10 @@
         </is>
       </c>
       <c r="C192" s="2">
-        <v>45199.8793277419</v>
+        <v>45200.8793277419</v>
       </c>
       <c r="D192">
-        <v>28.1</v>
+        <v>27.3</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -4343,10 +4316,10 @@
         </is>
       </c>
       <c r="C193" s="2">
-        <v>45210.28945402447</v>
+        <v>45207.28945402447</v>
       </c>
       <c r="D193">
-        <v>26.5</v>
+        <v>25.6</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -4364,7 +4337,7 @@
         </is>
       </c>
       <c r="C194" s="2">
-        <v>45164.5357799448</v>
+        <v>45162.5357799448</v>
       </c>
       <c r="D194">
         <v>26.9</v>
@@ -4385,7 +4358,7 @@
         </is>
       </c>
       <c r="C195" s="2">
-        <v>45128.11515279114</v>
+        <v>45131.11515279114</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -4406,7 +4379,7 @@
         <v>45130.21749240049</v>
       </c>
       <c r="D196">
-        <v>27</v>
+        <v>27.2</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -4424,10 +4397,10 @@
         </is>
       </c>
       <c r="C197" s="2">
-        <v>45125.05174723085</v>
+        <v>45126.05174723085</v>
       </c>
       <c r="D197">
-        <v>27.1</v>
+        <v>28</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -4445,10 +4418,10 @@
         </is>
       </c>
       <c r="C198" s="2">
-        <v>45134.01179841989</v>
+        <v>45136.01179841989</v>
       </c>
       <c r="D198">
-        <v>26.3</v>
+        <v>27.1</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -4487,10 +4460,10 @@
         </is>
       </c>
       <c r="C200" s="2">
-        <v>45162.32794732532</v>
+        <v>45159.32794732532</v>
       </c>
       <c r="D200">
-        <v>27.7</v>
+        <v>27.2</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -4511,7 +4484,7 @@
         <v>45154.98824595465</v>
       </c>
       <c r="D201">
-        <v>27.5</v>
+        <v>26.3</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -4529,10 +4502,10 @@
         </is>
       </c>
       <c r="C202" s="2">
-        <v>45163.87549791852</v>
+        <v>45164.87549791852</v>
       </c>
       <c r="D202">
-        <v>28.8</v>
+        <v>28.4</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -4568,10 +4541,10 @@
         </is>
       </c>
       <c r="C204" s="2">
-        <v>45171.17546254096</v>
+        <v>45174.17546254096</v>
       </c>
       <c r="D204">
-        <v>26.2</v>
+        <v>28.3</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -4589,10 +4562,10 @@
         </is>
       </c>
       <c r="C205" s="2">
-        <v>45165.26151633637</v>
+        <v>45164.26151633637</v>
       </c>
       <c r="D205">
-        <v>27.1</v>
+        <v>28.5</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -4613,7 +4586,7 @@
         <v>45112.46538148788</v>
       </c>
       <c r="D206">
-        <v>26.9</v>
+        <v>25.3</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -4631,10 +4604,10 @@
         </is>
       </c>
       <c r="C207" s="2">
-        <v>45104.51992590784</v>
+        <v>45103.51992590784</v>
       </c>
       <c r="D207">
-        <v>27.7</v>
+        <v>28.7</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -4654,9 +4627,12 @@
       <c r="C208" s="2">
         <v>45104.62946503496</v>
       </c>
+      <c r="D208">
+        <v>28.5</v>
+      </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -4670,14 +4646,11 @@
         </is>
       </c>
       <c r="C209" s="2">
-        <v>45127.38904542279</v>
-      </c>
-      <c r="D209">
-        <v>25.8</v>
+        <v>45129.38904542279</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -4691,11 +4664,14 @@
         </is>
       </c>
       <c r="C210" s="2">
-        <v>45161.74567539161</v>
+        <v>45164.74567539161</v>
+      </c>
+      <c r="D210">
+        <v>27.8</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -4712,7 +4688,7 @@
         <v>45175.48342637857</v>
       </c>
       <c r="D211">
-        <v>26.6</v>
+        <v>26.8</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -4730,10 +4706,10 @@
         </is>
       </c>
       <c r="C212" s="2">
-        <v>45174.67571837288</v>
+        <v>45172.67571837288</v>
       </c>
       <c r="D212">
-        <v>28.6</v>
+        <v>28.2</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -4751,10 +4727,10 @@
         </is>
       </c>
       <c r="C213" s="2">
-        <v>45104.78737318145</v>
+        <v>45105.78737318145</v>
       </c>
       <c r="D213">
-        <v>29.2</v>
+        <v>25.7</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -4772,11 +4748,14 @@
         </is>
       </c>
       <c r="C214" s="2">
-        <v>45106.19636170614</v>
+        <v>45108.19636170614</v>
+      </c>
+      <c r="D214">
+        <v>27.2</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -4792,9 +4771,12 @@
       <c r="C215" s="2">
         <v>45128.289470942</v>
       </c>
+      <c r="D215">
+        <v>29.5</v>
+      </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -4808,10 +4790,10 @@
         </is>
       </c>
       <c r="C216" s="2">
-        <v>45181.75459985403</v>
+        <v>45178.75459985403</v>
       </c>
       <c r="D216">
-        <v>28.4</v>
+        <v>26.8</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -4829,14 +4811,11 @@
         </is>
       </c>
       <c r="C217" s="2">
-        <v>45165.64088409244</v>
-      </c>
-      <c r="D217">
-        <v>26.8</v>
+        <v>45164.64088409244</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -4850,10 +4829,10 @@
         </is>
       </c>
       <c r="C218" s="2">
-        <v>45189.35888910964</v>
+        <v>45186.35888910964</v>
       </c>
       <c r="D218">
-        <v>27.9</v>
+        <v>27.2</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -4871,10 +4850,10 @@
         </is>
       </c>
       <c r="C219" s="2">
-        <v>45170.64360850202</v>
+        <v>45171.64360850202</v>
       </c>
       <c r="D219">
-        <v>27.8</v>
+        <v>28.9</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -4892,10 +4871,10 @@
         </is>
       </c>
       <c r="C220" s="2">
-        <v>45172.2595007636</v>
+        <v>45171.2595007636</v>
       </c>
       <c r="D220">
-        <v>29.2</v>
+        <v>27.8</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -4916,7 +4895,7 @@
         <v>45181.83381148289</v>
       </c>
       <c r="D221">
-        <v>25.4</v>
+        <v>27.2</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -4937,7 +4916,7 @@
         <v>45128.55459567619</v>
       </c>
       <c r="D222">
-        <v>28.2</v>
+        <v>25.9</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -4958,7 +4937,7 @@
         <v>45119.41272913327</v>
       </c>
       <c r="D223">
-        <v>28.4</v>
+        <v>27.9</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -4976,14 +4955,11 @@
         </is>
       </c>
       <c r="C224" s="2">
-        <v>45109.83177388464</v>
-      </c>
-      <c r="D224">
-        <v>26.6</v>
+        <v>45107.83177388464</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -5000,7 +4976,7 @@
         <v>45133.0060951889</v>
       </c>
       <c r="D225">
-        <v>27.2</v>
+        <v>26</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5018,10 +4994,10 @@
         </is>
       </c>
       <c r="C226" s="2">
-        <v>45188.47050502237</v>
+        <v>45186.47050502237</v>
       </c>
       <c r="D226">
-        <v>27.5</v>
+        <v>25.7</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -5041,12 +5017,9 @@
       <c r="C227" s="2">
         <v>45185.14749938398</v>
       </c>
-      <c r="D227">
-        <v>28</v>
-      </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -5060,11 +5033,14 @@
         </is>
       </c>
       <c r="C228" s="2">
-        <v>45168.34568989</v>
+        <v>45170.34568989</v>
+      </c>
+      <c r="D228">
+        <v>28</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -5078,10 +5054,10 @@
         </is>
       </c>
       <c r="C229" s="2">
-        <v>45160.96805144587</v>
+        <v>45158.96805144587</v>
       </c>
       <c r="D229">
-        <v>26.5</v>
+        <v>27</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -5101,12 +5077,9 @@
       <c r="C230" s="2">
         <v>45197.0299278239</v>
       </c>
-      <c r="D230">
-        <v>27.1</v>
-      </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -5120,10 +5093,10 @@
         </is>
       </c>
       <c r="C231" s="2">
-        <v>45196.65662753381</v>
+        <v>45197.65662753381</v>
       </c>
       <c r="D231">
-        <v>28.6</v>
+        <v>26.7</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -5144,7 +5117,7 @@
         <v>45189.98498173171</v>
       </c>
       <c r="D232">
-        <v>27.1</v>
+        <v>27</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -5162,14 +5135,11 @@
         </is>
       </c>
       <c r="C233" s="2">
-        <v>45136.83640703386</v>
-      </c>
-      <c r="D233">
-        <v>27.3</v>
+        <v>45137.83640703386</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -5183,10 +5153,10 @@
         </is>
       </c>
       <c r="C234" s="2">
-        <v>45139.67293091925</v>
+        <v>45138.67293091925</v>
       </c>
       <c r="D234">
-        <v>29.1</v>
+        <v>26</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -5206,12 +5176,9 @@
       <c r="C235" s="2">
         <v>45140.28923538393</v>
       </c>
-      <c r="D235">
-        <v>28.3</v>
-      </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -5225,14 +5192,11 @@
         </is>
       </c>
       <c r="C236" s="2">
-        <v>45194.71736660851</v>
-      </c>
-      <c r="D236">
-        <v>28.3</v>
+        <v>45196.71736660851</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -5246,10 +5210,10 @@
         </is>
       </c>
       <c r="C237" s="2">
-        <v>45190.35861425864</v>
+        <v>45191.35861425864</v>
       </c>
       <c r="D237">
-        <v>26.3</v>
+        <v>27</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -5267,10 +5231,10 @@
         </is>
       </c>
       <c r="C238" s="2">
-        <v>45163.69841918358</v>
+        <v>45165.69841918358</v>
       </c>
       <c r="D238">
-        <v>27.1</v>
+        <v>27</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -5291,7 +5255,7 @@
         <v>45178.53717435489</v>
       </c>
       <c r="D239">
-        <v>27.5</v>
+        <v>26.1</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -5311,12 +5275,9 @@
       <c r="C240" s="2">
         <v>45200.36995174419</v>
       </c>
-      <c r="D240">
-        <v>27.7</v>
-      </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -5330,10 +5291,10 @@
         </is>
       </c>
       <c r="C241" s="2">
-        <v>45188.47605414721</v>
+        <v>45189.47605414721</v>
       </c>
       <c r="D241">
-        <v>28</v>
+        <v>28.4</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -5351,14 +5312,11 @@
         </is>
       </c>
       <c r="C242" s="2">
-        <v>45140.39351033657</v>
-      </c>
-      <c r="D242">
-        <v>28.5</v>
+        <v>45139.39351033657</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -5372,11 +5330,14 @@
         </is>
       </c>
       <c r="C243" s="2">
-        <v>45152.45384713256</v>
+        <v>45151.45384713256</v>
+      </c>
+      <c r="D243">
+        <v>26.2</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -5390,10 +5351,10 @@
         </is>
       </c>
       <c r="C244" s="2">
-        <v>45152.41921885805</v>
+        <v>45150.41921885805</v>
       </c>
       <c r="D244">
-        <v>26.6</v>
+        <v>28.4</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -5411,10 +5372,10 @@
         </is>
       </c>
       <c r="C245" s="2">
-        <v>45143.46369356522</v>
+        <v>45145.46369356522</v>
       </c>
       <c r="D245">
-        <v>27.6</v>
+        <v>28.5</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -5432,14 +5393,11 @@
         </is>
       </c>
       <c r="C246" s="2">
-        <v>45173.79834337314</v>
-      </c>
-      <c r="D246">
-        <v>27.7</v>
+        <v>45174.79834337314</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -5453,10 +5411,10 @@
         </is>
       </c>
       <c r="C247" s="2">
-        <v>45195.65724226883</v>
+        <v>45192.65724226883</v>
       </c>
       <c r="D247">
-        <v>26.8</v>
+        <v>25.4</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -5476,12 +5434,9 @@
       <c r="C248" s="2">
         <v>45137.41705280713</v>
       </c>
-      <c r="D248">
-        <v>26.7</v>
-      </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -5495,10 +5450,10 @@
         </is>
       </c>
       <c r="C249" s="2">
-        <v>45155.10940375135</v>
+        <v>45153.10940375135</v>
       </c>
       <c r="D249">
-        <v>29</v>
+        <v>26.3</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -5516,11 +5471,11 @@
         </is>
       </c>
       <c r="C250" s="2">
-        <v>45157.77375944021</v>
+        <v>45156.77375944021</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -5534,10 +5489,10 @@
         </is>
       </c>
       <c r="C251" s="2">
-        <v>45202.91169867139</v>
+        <v>45204.91169867139</v>
       </c>
       <c r="D251">
-        <v>28.3</v>
+        <v>25.6</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -5558,7 +5513,7 @@
         <v>45205.36572316945</v>
       </c>
       <c r="D252">
-        <v>26.2</v>
+        <v>27.7</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -5576,10 +5531,10 @@
         </is>
       </c>
       <c r="C253" s="2">
-        <v>45194.40795615399</v>
+        <v>45195.40795615399</v>
       </c>
       <c r="D253">
-        <v>27.3</v>
+        <v>26.8</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -5600,7 +5555,7 @@
         <v>45191.228278898</v>
       </c>
       <c r="D254">
-        <v>27.7</v>
+        <v>29.2</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -5618,14 +5573,11 @@
         </is>
       </c>
       <c r="C255" s="2">
-        <v>45186.62400840544</v>
-      </c>
-      <c r="D255">
-        <v>25.2</v>
+        <v>45187.62400840544</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -5641,9 +5593,12 @@
       <c r="C256" s="2">
         <v>45176.87060432407</v>
       </c>
+      <c r="D256">
+        <v>28.3</v>
+      </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -5657,14 +5612,11 @@
         </is>
       </c>
       <c r="C257" s="2">
-        <v>45208.09525342345</v>
-      </c>
-      <c r="D257">
-        <v>28.6</v>
+        <v>45206.09525342345</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -5678,11 +5630,14 @@
         </is>
       </c>
       <c r="C258" s="2">
-        <v>45188.58552653385</v>
+        <v>45189.58552653385</v>
+      </c>
+      <c r="D258">
+        <v>25.9</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -5696,7 +5651,7 @@
         </is>
       </c>
       <c r="C259" s="2">
-        <v>45186.75726822948</v>
+        <v>45187.75726822948</v>
       </c>
       <c r="D259">
         <v>27.5</v>
@@ -5717,14 +5672,11 @@
         </is>
       </c>
       <c r="C260" s="2">
-        <v>45181.39516517524</v>
-      </c>
-      <c r="D260">
-        <v>28.7</v>
+        <v>45180.39516517524</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -5738,10 +5690,10 @@
         </is>
       </c>
       <c r="C261" s="2">
-        <v>45134.13537434634</v>
+        <v>45136.13537434634</v>
       </c>
       <c r="D261">
-        <v>28.4</v>
+        <v>26.5</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -5759,10 +5711,10 @@
         </is>
       </c>
       <c r="C262" s="2">
-        <v>45147.97883870429</v>
+        <v>45149.97883870429</v>
       </c>
       <c r="D262">
-        <v>28.1</v>
+        <v>27.5</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -5782,12 +5734,9 @@
       <c r="C263" s="2">
         <v>45150.7782290528</v>
       </c>
-      <c r="D263">
-        <v>26.8</v>
-      </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -5804,7 +5753,7 @@
         <v>45165.65233913012</v>
       </c>
       <c r="D264">
-        <v>25.7</v>
+        <v>28.1</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -5822,10 +5771,10 @@
         </is>
       </c>
       <c r="C265" s="2">
-        <v>45173.9498169107</v>
+        <v>45170.9498169107</v>
       </c>
       <c r="D265">
-        <v>27.2</v>
+        <v>25.5</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -5843,14 +5792,11 @@
         </is>
       </c>
       <c r="C266" s="2">
-        <v>45142.33078768222</v>
-      </c>
-      <c r="D266">
-        <v>27.4</v>
+        <v>45143.33078768222</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -5867,7 +5813,7 @@
         <v>45148.27830788869</v>
       </c>
       <c r="D267">
-        <v>26.7</v>
+        <v>27.3</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -5885,10 +5831,10 @@
         </is>
       </c>
       <c r="C268" s="2">
-        <v>45206.8879070961</v>
+        <v>45205.8879070961</v>
       </c>
       <c r="D268">
-        <v>28.5</v>
+        <v>26.4</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -5906,10 +5852,10 @@
         </is>
       </c>
       <c r="C269" s="2">
-        <v>45192.60112519143</v>
+        <v>45195.60112519143</v>
       </c>
       <c r="D269">
-        <v>29.1</v>
+        <v>26.7</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -5927,10 +5873,10 @@
         </is>
       </c>
       <c r="C270" s="2">
-        <v>45209.39906610698</v>
+        <v>45208.39906610698</v>
       </c>
       <c r="D270">
-        <v>28.8</v>
+        <v>25.7</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -5948,10 +5894,10 @@
         </is>
       </c>
       <c r="C271" s="2">
-        <v>45219.32990988754</v>
+        <v>45218.32990988754</v>
       </c>
       <c r="D271">
-        <v>28.6</v>
+        <v>26.2</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -5969,11 +5915,14 @@
         </is>
       </c>
       <c r="C272" s="2">
-        <v>45209.49579965682</v>
+        <v>45208.49579965682</v>
+      </c>
+      <c r="D272">
+        <v>27</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -5987,10 +5936,10 @@
         </is>
       </c>
       <c r="C273" s="2">
-        <v>45194.0668039692</v>
+        <v>45196.0668039692</v>
       </c>
       <c r="D273">
-        <v>27.3</v>
+        <v>26.7</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -6008,10 +5957,10 @@
         </is>
       </c>
       <c r="C274" s="2">
-        <v>45142.39240210949</v>
+        <v>45143.39240210949</v>
       </c>
       <c r="D274">
-        <v>28.3</v>
+        <v>26.6</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -6029,10 +5978,10 @@
         </is>
       </c>
       <c r="C275" s="2">
-        <v>45171.34052446077</v>
+        <v>45169.34052446077</v>
       </c>
       <c r="D275">
-        <v>29.5</v>
+        <v>27.9</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -6050,10 +5999,10 @@
         </is>
       </c>
       <c r="C276" s="2">
-        <v>45201.67379095823</v>
+        <v>45200.67379095823</v>
       </c>
       <c r="D276">
-        <v>26</v>
+        <v>27.6</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -6071,10 +6020,10 @@
         </is>
       </c>
       <c r="C277" s="2">
-        <v>45224.7629075281</v>
+        <v>45223.7629075281</v>
       </c>
       <c r="D277">
-        <v>26.9</v>
+        <v>27.9</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -6092,10 +6041,10 @@
         </is>
       </c>
       <c r="C278" s="2">
-        <v>45190.72006929193</v>
+        <v>45191.72006929193</v>
       </c>
       <c r="D278">
-        <v>26.1</v>
+        <v>27.6</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -6113,10 +6062,10 @@
         </is>
       </c>
       <c r="C279" s="2">
-        <v>45218.05618489677</v>
+        <v>45219.05618489677</v>
       </c>
       <c r="D279">
-        <v>28.6</v>
+        <v>27.1</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -6134,11 +6083,14 @@
         </is>
       </c>
       <c r="C280" s="2">
-        <v>45212.41157251294</v>
+        <v>45210.41157251294</v>
+      </c>
+      <c r="D280">
+        <v>28</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -6152,10 +6104,10 @@
         </is>
       </c>
       <c r="C281" s="2">
-        <v>45205.34713681876</v>
+        <v>45208.34713681876</v>
       </c>
       <c r="D281">
-        <v>27.2</v>
+        <v>27.1</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -6176,7 +6128,7 @@
         <v>45146.83201890838</v>
       </c>
       <c r="D282">
-        <v>26</v>
+        <v>27.3</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -6194,10 +6146,10 @@
         </is>
       </c>
       <c r="C283" s="2">
-        <v>45143.09624968136</v>
+        <v>45144.09624968136</v>
       </c>
       <c r="D283">
-        <v>25.8</v>
+        <v>26.8</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -6215,10 +6167,10 @@
         </is>
       </c>
       <c r="C284" s="2">
-        <v>45152.71171535416</v>
+        <v>45150.71171535416</v>
       </c>
       <c r="D284">
-        <v>26.3</v>
+        <v>27.4</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -6236,11 +6188,14 @@
         </is>
       </c>
       <c r="C285" s="2">
-        <v>45166.49748360754</v>
+        <v>45165.49748360754</v>
+      </c>
+      <c r="D285">
+        <v>28.4</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -6254,10 +6209,10 @@
         </is>
       </c>
       <c r="C286" s="2">
-        <v>45153.75517243127</v>
+        <v>45154.75517243127</v>
       </c>
       <c r="D286">
-        <v>28.4</v>
+        <v>27.2</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -6277,9 +6232,12 @@
       <c r="C287" s="2">
         <v>45178.35780207686</v>
       </c>
+      <c r="D287">
+        <v>26.1</v>
+      </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -6296,7 +6254,7 @@
         <v>45162.37326743235</v>
       </c>
       <c r="D288">
-        <v>27.5</v>
+        <v>28.5</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -6314,10 +6272,10 @@
         </is>
       </c>
       <c r="C289" s="2">
-        <v>45165.38359012485</v>
+        <v>45164.38359012485</v>
       </c>
       <c r="D289">
-        <v>26.2</v>
+        <v>28.3</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -6337,12 +6295,9 @@
       <c r="C290" s="2">
         <v>45204.48383897445</v>
       </c>
-      <c r="D290">
-        <v>25.6</v>
-      </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -6356,10 +6311,10 @@
         </is>
       </c>
       <c r="C291" s="2">
-        <v>45214.04477986079</v>
+        <v>45211.04477986079</v>
       </c>
       <c r="D291">
-        <v>27.6</v>
+        <v>26.6</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -6380,7 +6335,7 @@
         <v>45228.0433442397</v>
       </c>
       <c r="D292">
-        <v>26.9</v>
+        <v>27.3</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -6398,10 +6353,10 @@
         </is>
       </c>
       <c r="C293" s="2">
-        <v>45204.23483707381</v>
+        <v>45205.23483707381</v>
       </c>
       <c r="D293">
-        <v>26.9</v>
+        <v>28.6</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -6419,10 +6374,10 @@
         </is>
       </c>
       <c r="C294" s="2">
-        <v>45211.63077185371</v>
+        <v>45210.63077185371</v>
       </c>
       <c r="D294">
-        <v>26.8</v>
+        <v>27.3</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -6440,11 +6395,14 @@
         </is>
       </c>
       <c r="C295" s="2">
-        <v>45215.5606938148</v>
+        <v>45214.5606938148</v>
+      </c>
+      <c r="D295">
+        <v>27.2</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -6460,12 +6418,9 @@
       <c r="C296" s="2">
         <v>45213.38935128621</v>
       </c>
-      <c r="D296">
-        <v>25.8</v>
-      </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -6479,10 +6434,10 @@
         </is>
       </c>
       <c r="C297" s="2">
-        <v>45203.8304463174</v>
+        <v>45205.8304463174</v>
       </c>
       <c r="D297">
-        <v>26.7</v>
+        <v>26</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -6503,7 +6458,7 @@
         <v>45205.82375632683</v>
       </c>
       <c r="D298">
-        <v>27.8</v>
+        <v>27.7</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -6524,7 +6479,7 @@
         <v>45207.95402109734</v>
       </c>
       <c r="D299">
-        <v>28.9</v>
+        <v>27.6</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -6542,14 +6497,11 @@
         </is>
       </c>
       <c r="C300" s="2">
-        <v>45157.13707859364</v>
-      </c>
-      <c r="D300">
-        <v>27.6</v>
+        <v>45160.13707859364</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>inconclusive</t>
         </is>
       </c>
     </row>
@@ -6563,10 +6515,10 @@
         </is>
       </c>
       <c r="C301" s="2">
-        <v>45161.3552429834</v>
+        <v>45160.3552429834</v>
       </c>
       <c r="D301">
-        <v>27.3</v>
+        <v>26.7</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -6584,10 +6536,10 @@
         </is>
       </c>
       <c r="C302" s="2">
-        <v>45175.23549482663</v>
+        <v>45174.23549482663</v>
       </c>
       <c r="D302">
-        <v>26.6</v>
+        <v>27.3</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -6605,10 +6557,10 @@
         </is>
       </c>
       <c r="C303" s="2">
-        <v>45152.02117476883</v>
+        <v>45153.02117476883</v>
       </c>
       <c r="D303">
-        <v>27.5</v>
+        <v>28.4</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -6629,7 +6581,7 @@
         <v>45171.25602206562</v>
       </c>
       <c r="D304">
-        <v>27.2</v>
+        <v>28.5</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -6650,7 +6602,7 @@
         <v>45209.42443018156</v>
       </c>
       <c r="D305">
-        <v>27.4</v>
+        <v>26.8</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -6671,7 +6623,7 @@
         <v>45203.20656796377</v>
       </c>
       <c r="D306">
-        <v>28.6</v>
+        <v>27</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -6689,10 +6641,10 @@
         </is>
       </c>
       <c r="C307" s="2">
-        <v>45225.75889984527</v>
+        <v>45224.75889984527</v>
       </c>
       <c r="D307">
-        <v>26.1</v>
+        <v>26.3</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -6710,11 +6662,14 @@
         </is>
       </c>
       <c r="C308" s="2">
-        <v>45218.74777502281</v>
+        <v>45217.74777502281</v>
+      </c>
+      <c r="D308">
+        <v>26.9</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -6728,10 +6683,10 @@
         </is>
       </c>
       <c r="C309" s="2">
-        <v>45200.067767916</v>
+        <v>45199.067767916</v>
       </c>
       <c r="D309">
-        <v>26.9</v>
+        <v>27.3</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -6749,10 +6704,10 @@
         </is>
       </c>
       <c r="C310" s="2">
-        <v>45221.25660068549</v>
+        <v>45224.25660068549</v>
       </c>
       <c r="D310">
-        <v>28.3</v>
+        <v>26</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -6770,10 +6725,10 @@
         </is>
       </c>
       <c r="C311" s="2">
-        <v>45174.6282028081</v>
+        <v>45176.6282028081</v>
       </c>
       <c r="D311">
-        <v>28.8</v>
+        <v>27</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -6794,7 +6749,7 @@
         <v>45159.46753103727</v>
       </c>
       <c r="D312">
-        <v>27</v>
+        <v>28.6</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -6814,9 +6769,12 @@
       <c r="C313" s="2">
         <v>45181.41041761494</v>
       </c>
+      <c r="D313">
+        <v>27.4</v>
+      </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -6830,10 +6788,10 @@
         </is>
       </c>
       <c r="C314" s="2">
-        <v>45234.67042588619</v>
+        <v>45236.67042588619</v>
       </c>
       <c r="D314">
-        <v>27.8</v>
+        <v>26.4</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -6851,10 +6809,10 @@
         </is>
       </c>
       <c r="C315" s="2">
-        <v>45205.75786535986</v>
+        <v>45204.75786535986</v>
       </c>
       <c r="D315">
-        <v>27.5</v>
+        <v>27.8</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -6872,11 +6830,14 @@
         </is>
       </c>
       <c r="C316" s="2">
-        <v>45211.21301142181</v>
+        <v>45210.21301142181</v>
+      </c>
+      <c r="D316">
+        <v>26.4</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>inconclusive</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -6908,10 +6869,10 @@
         </is>
       </c>
       <c r="C318" s="2">
-        <v>45231.72395626019</v>
+        <v>45233.72395626019</v>
       </c>
       <c r="D318">
-        <v>28.6</v>
+        <v>26.6</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -6929,10 +6890,10 @@
         </is>
       </c>
       <c r="C319" s="2">
-        <v>45204.46181093609</v>
+        <v>45202.46181093609</v>
       </c>
       <c r="D319">
-        <v>27.9</v>
+        <v>28.1</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -6953,7 +6914,7 @@
         <v>45232.46348036611</v>
       </c>
       <c r="D320">
-        <v>26.5</v>
+        <v>28.1</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -6971,10 +6932,10 @@
         </is>
       </c>
       <c r="C321" s="2">
-        <v>45211.78604913782</v>
+        <v>45210.78604913782</v>
       </c>
       <c r="D321">
-        <v>26.6</v>
+        <v>27.4</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -6992,10 +6953,10 @@
         </is>
       </c>
       <c r="C322" s="2">
-        <v>45203.49394192699</v>
+        <v>45205.49394192699</v>
       </c>
       <c r="D322">
-        <v>27.2</v>
+        <v>26.1</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -7013,10 +6974,10 @@
         </is>
       </c>
       <c r="C323" s="2">
-        <v>45192.32979394906</v>
+        <v>45193.32979394906</v>
       </c>
       <c r="D323">
-        <v>27.5</v>
+        <v>28.4</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -7034,10 +6995,10 @@
         </is>
       </c>
       <c r="C324" s="2">
-        <v>45232.01866285874</v>
+        <v>45235.01866285874</v>
       </c>
       <c r="D324">
-        <v>28</v>
+        <v>26.1</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -7058,7 +7019,7 @@
         <v>45230.95418620377</v>
       </c>
       <c r="D325">
-        <v>27</v>
+        <v>28.1</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -7079,7 +7040,7 @@
         <v>45220.0120123856</v>
       </c>
       <c r="D326">
-        <v>26.3</v>
+        <v>26.4</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -7100,7 +7061,7 @@
         <v>45254.1086374196</v>
       </c>
       <c r="D327">
-        <v>26.8</v>
+        <v>26.7</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -7121,7 +7082,7 @@
         <v>45226.78925026321</v>
       </c>
       <c r="D328">
-        <v>27.1</v>
+        <v>27.6</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -7142,7 +7103,7 @@
         <v>45232.08599691609</v>
       </c>
       <c r="D329">
-        <v>27.6</v>
+        <v>28</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -7160,10 +7121,10 @@
         </is>
       </c>
       <c r="C330" s="2">
-        <v>45219.82938611381</v>
+        <v>45218.82938611381</v>
       </c>
       <c r="D330">
-        <v>27.6</v>
+        <v>27.2</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -7173,57 +7134,57 @@
     </row>
     <row r="331">
       <c r="A331">
-        <v>1470</v>
+        <v>1050</v>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>BOU-11_retest</t>
+          <t>BOU-4_retest</t>
         </is>
       </c>
       <c r="C331" s="2">
-        <v>44988.22862544721</v>
+        <v>44971.19165913553</v>
+      </c>
+      <c r="D331">
+        <v>28.02202123572184</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332">
-        <v>1978</v>
+        <v>1106</v>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>MOI-50_retest</t>
+          <t>BOU-5_retest</t>
         </is>
       </c>
       <c r="C332" s="2">
-        <v>45015.51728321377</v>
-      </c>
-      <c r="D332">
-        <v>26.7197893940301</v>
+        <v>44967.45561075702</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333">
-        <v>2060</v>
+        <v>1953</v>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>BOU-19_retest</t>
+          <t>MOI-49_retest</t>
         </is>
       </c>
       <c r="C333" s="2">
-        <v>45023.68565493632</v>
+        <v>45009.18506884721</v>
       </c>
       <c r="D333">
-        <v>27.81400799664609</v>
+        <v>29.29813880690743</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -7233,18 +7194,18 @@
     </row>
     <row r="334">
       <c r="A334">
-        <v>2647</v>
+        <v>2141</v>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>BOU-29_retest</t>
+          <t>MOI-52_retest</t>
         </is>
       </c>
       <c r="C334" s="2">
-        <v>45046.44525145847</v>
+        <v>45031.75037402037</v>
       </c>
       <c r="D334">
-        <v>26.31680675129488</v>
+        <v>27.44980094450562</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -7254,39 +7215,36 @@
     </row>
     <row r="335">
       <c r="A335">
-        <v>3227</v>
+        <v>2632</v>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>BOU-35_retest</t>
+          <t>MOI-66_retest</t>
         </is>
       </c>
       <c r="C335" s="2">
-        <v>45067.67696978927</v>
-      </c>
-      <c r="D335">
-        <v>27.4985538739235</v>
+        <v>45019.90476873251</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336">
-        <v>3328</v>
+        <v>3471</v>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>BOU-37_retest</t>
+          <t>BOU-40_retest</t>
         </is>
       </c>
       <c r="C336" s="2">
-        <v>45056.97612192866</v>
+        <v>45082.29387128746</v>
       </c>
       <c r="D336">
-        <v>26.58074734145184</v>
+        <v>27.11781648632729</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -7296,18 +7254,18 @@
     </row>
     <row r="337">
       <c r="A337">
-        <v>3458</v>
+        <v>4592</v>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>MOI-82_retest</t>
+          <t>MOI-94_retest</t>
         </is>
       </c>
       <c r="C337" s="2">
-        <v>45066.57257599347</v>
+        <v>45113.96701374761</v>
       </c>
       <c r="D337">
-        <v>28.88428292180577</v>
+        <v>25.86615926260534</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -7317,18 +7275,18 @@
     </row>
     <row r="338">
       <c r="A338">
-        <v>4261</v>
+        <v>4603</v>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>BEK-2_retest</t>
+          <t>MOI-95_retest</t>
         </is>
       </c>
       <c r="C338" s="2">
-        <v>45111.33771034843</v>
+        <v>45128.17916409774</v>
       </c>
       <c r="D338">
-        <v>27.2673887051399</v>
+        <v>26.45525992648956</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -7338,18 +7296,18 @@
     </row>
     <row r="339">
       <c r="A339">
-        <v>4398</v>
+        <v>5554</v>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>MOI-91_retest</t>
+          <t>BED-10_retest</t>
         </is>
       </c>
       <c r="C339" s="2">
-        <v>45132.40256878556</v>
+        <v>45149.91435035678</v>
       </c>
       <c r="D339">
-        <v>26.20291151848792</v>
+        <v>27.77357679339763</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -7359,39 +7317,36 @@
     </row>
     <row r="340">
       <c r="A340">
-        <v>5461</v>
+        <v>5560</v>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>BEK-12_retest</t>
+          <t>BOU-58_retest</t>
         </is>
       </c>
       <c r="C340" s="2">
-        <v>45112.57957767218</v>
-      </c>
-      <c r="D340">
-        <v>27.18523314404388</v>
+        <v>45154.35639856065</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341">
-        <v>5855</v>
+        <v>5739</v>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>BED-14_retest</t>
+          <t>MOI-101_retest</t>
         </is>
       </c>
       <c r="C341" s="2">
-        <v>45130.11515279114</v>
+        <v>45151.96254063725</v>
       </c>
       <c r="D341">
-        <v>26.220500493255</v>
+        <v>27.63296573816749</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -7401,18 +7356,18 @@
     </row>
     <row r="342">
       <c r="A342">
-        <v>6109</v>
+        <v>5855</v>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>BED-21_retest</t>
+          <t>BED-14_retest</t>
         </is>
       </c>
       <c r="C342" s="2">
-        <v>45105.62946503496</v>
+        <v>45133.11515279114</v>
       </c>
       <c r="D342">
-        <v>27.73147509750649</v>
+        <v>28.77447197229267</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -7422,18 +7377,18 @@
     </row>
     <row r="343">
       <c r="A343">
-        <v>6162</v>
+        <v>6126</v>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>GOU-2_retest</t>
+          <t>BED-22_retest</t>
         </is>
       </c>
       <c r="C343" s="2">
-        <v>45165.74567539161</v>
+        <v>45132.38904542279</v>
       </c>
       <c r="D343">
-        <v>26.65984323306497</v>
+        <v>29.01788362360979</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -7443,18 +7398,18 @@
     </row>
     <row r="344">
       <c r="A344">
-        <v>7297</v>
+        <v>6452</v>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>BEK-24_retest</t>
+          <t>BED-25_retest</t>
         </is>
       </c>
       <c r="C344" s="2">
-        <v>45156.45384713256</v>
+        <v>45168.64088409244</v>
       </c>
       <c r="D344">
-        <v>27.64027605559749</v>
+        <v>28.63050644816769</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -7464,15 +7419,15 @@
     </row>
     <row r="345">
       <c r="A345">
-        <v>7665</v>
+        <v>6761</v>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>MOI-107_retest</t>
+          <t>BED-30_retest</t>
         </is>
       </c>
       <c r="C345" s="2">
-        <v>45159.77375944021</v>
+        <v>45188.14749938398</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -7482,18 +7437,18 @@
     </row>
     <row r="346">
       <c r="A346">
-        <v>8812</v>
+        <v>7059</v>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>KOU-11_retest</t>
+          <t>BED-34_retest</t>
         </is>
       </c>
       <c r="C346" s="2">
-        <v>45217.5606938148</v>
+        <v>45199.71736660851</v>
       </c>
       <c r="D346">
-        <v>27.5125356488794</v>
+        <v>28.29743651590875</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -7503,38 +7458,119 @@
     </row>
     <row r="347">
       <c r="A347">
-        <v>9108</v>
+        <v>7178</v>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>BEK-33_retest</t>
+          <t>BOU-67_retest</t>
         </is>
       </c>
       <c r="C347" s="2">
-        <v>45222.74777502281</v>
+        <v>45201.36995174419</v>
+      </c>
+      <c r="D347">
+        <v>26.28961943047275</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348">
-        <v>9405</v>
+        <v>7233</v>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>BEK-36_retest</t>
+          <t>BEK-23_retest</t>
         </is>
       </c>
       <c r="C348" s="2">
-        <v>45214.21301142181</v>
-      </c>
-      <c r="D348">
-        <v>27.93569468466389</v>
+        <v>45141.39351033657</v>
       </c>
       <c r="E348" t="inlineStr">
+        <is>
+          <t>inconclusive</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349">
+        <v>7572</v>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>BED-37_retest</t>
+        </is>
+      </c>
+      <c r="C349" s="2">
+        <v>45138.41705280713</v>
+      </c>
+      <c r="D349">
+        <v>28.40796651202638</v>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350">
+        <v>8002</v>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>MOI-112_retest</t>
+        </is>
+      </c>
+      <c r="C350" s="2">
+        <v>45145.33078768222</v>
+      </c>
+      <c r="D350">
+        <v>27.06381540092295</v>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351">
+        <v>8699</v>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>BEK-29_retest</t>
+        </is>
+      </c>
+      <c r="C351" s="2">
+        <v>45208.48383897445</v>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352">
+        <v>8897</v>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>BEK-30_retest</t>
+        </is>
+      </c>
+      <c r="C352" s="2">
+        <v>45164.13707859364</v>
+      </c>
+      <c r="D352">
+        <v>26.23368351897652</v>
+      </c>
+      <c r="E352" t="inlineStr">
         <is>
           <t>positive</t>
         </is>

</xml_diff>